<commit_message>
Added "needs more investigation" to empty fields in Curated-Dataset-Slim_2025-04-18.xlsx
</commit_message>
<xml_diff>
--- a/Datasets/Curated-Dataset-Slim_2025-04-18.xlsx
+++ b/Datasets/Curated-Dataset-Slim_2025-04-18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertopiranamedi/RiderProjects/Pulumissues/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3039B04B-9832-A244-964B-F61359B2B40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1ACA9-69E0-7440-B833-1D52A6BB812F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="42000" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="461">
   <si>
     <t>Url</t>
   </si>
@@ -3435,6 +3435,9 @@
   </si>
   <si>
     <t>ProTI does not access stack configuration nor generate its own values for [Pulumi's configuration mechanism](https://www.pulumi.com/docs/concepts/config/). We should add an interface to generator plugins to generate accessed configuration values.</t>
+  </si>
+  <si>
+    <t>Needs more investigation</t>
   </si>
 </sst>
 </file>
@@ -3728,10 +3731,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="F100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3744,9 +3747,10 @@
     <col min="6" max="6" width="255" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +3776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="234" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="234" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3798,7 +3802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3850,7 +3854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -3876,7 +3880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -3921,10 +3925,17 @@
       <c r="F7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -3950,7 +3961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="108" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="108" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -3976,7 +3987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="216" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="216" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -4002,7 +4013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -4028,7 +4039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="216" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="216" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -4054,7 +4065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -4080,7 +4091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -4106,7 +4117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
@@ -4132,7 +4143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
@@ -5380,7 +5391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>203</v>
       </c>
@@ -5406,7 +5417,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>206</v>
       </c>
@@ -5432,7 +5443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>209</v>
       </c>
@@ -5458,7 +5469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>212</v>
       </c>
@@ -5484,7 +5495,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>215</v>
       </c>
@@ -5510,7 +5521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>218</v>
       </c>
@@ -5536,7 +5547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>221</v>
       </c>
@@ -5562,7 +5573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>224</v>
       </c>
@@ -5588,7 +5599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>227</v>
       </c>
@@ -5614,7 +5625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>230</v>
       </c>
@@ -5640,7 +5651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>233</v>
       </c>
@@ -5666,7 +5677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>236</v>
       </c>
@@ -5692,7 +5703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>239</v>
       </c>
@@ -5718,7 +5729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>242</v>
       </c>
@@ -5744,7 +5755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>245</v>
       </c>
@@ -5770,7 +5781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>248</v>
       </c>
@@ -5796,7 +5807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>251</v>
       </c>
@@ -5820,6 +5831,9 @@
       </c>
       <c r="H80" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="342" hidden="1" x14ac:dyDescent="0.2">
@@ -6813,7 +6827,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7797,7 +7811,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>

</xml_diff>